<commit_message>
changed BSD license to Apache 2.0 license
</commit_message>
<xml_diff>
--- a/constrained_ik/test/puma_560_jacobian.xlsx
+++ b/constrained_ik/test/puma_560_jacobian.xlsx
@@ -8,14 +8,15 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="176" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ForwardKinematics" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="License" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
   <si>
     <t>Axis Angles</t>
   </si>
@@ -210,6 +211,111 @@
   </si>
   <si>
     <t>Rotation matrix (check on AA)</t>
+  </si>
+  <si>
+    <t>/*</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> * Software License Agreement (</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <color rgb="003F7F5F"/>
+        <sz val="10"/>
+        <u val="single"/>
+      </rPr>
+      <t xml:space="preserve">Apache</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </rPr>
+      <t xml:space="preserve"> License)</t>
+    </r>
+  </si>
+  <si>
+    <t> *</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> * Copyright (c) 2013, </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <color rgb="003F7F5F"/>
+        <sz val="10"/>
+        <u val="single"/>
+      </rPr>
+      <t xml:space="preserve">Southwest</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </rPr>
+      <t xml:space="preserve"> Research Institute</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> * Licensed under the </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Monospace"/>
+        <family val="0"/>
+        <color rgb="003F7F5F"/>
+        <sz val="10"/>
+        <u val="single"/>
+      </rPr>
+      <t xml:space="preserve">Apache</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </rPr>
+      <t xml:space="preserve"> License, Version 2.0 (the "License");</t>
+    </r>
+  </si>
+  <si>
+    <t> * you may not use this file except in compliance with the License.</t>
+  </si>
+  <si>
+    <t> * You may obtain a copy of the License at</t>
+  </si>
+  <si>
+    <t> *   http://www.apache.org/licenses/LICENSE-2.0</t>
+  </si>
+  <si>
+    <t> * Unless required by applicable law or agreed to in writing, software</t>
+  </si>
+  <si>
+    <t> * distributed under the License is distributed on an "AS IS" BASIS,</t>
+  </si>
+  <si>
+    <t> * WITHOUT WARRANTIES OR CONDITIONS OF ANY KIND, either express or implied.</t>
+  </si>
+  <si>
+    <t> * See the License for the specific language governing permissions and</t>
+  </si>
+  <si>
+    <t> * limitations under the License.</t>
+  </si>
+  <si>
+    <t> */</t>
   </si>
 </sst>
 </file>
@@ -223,7 +329,7 @@
     <numFmt formatCode="0.0000" numFmtId="167"/>
     <numFmt formatCode="0" numFmtId="168"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -259,6 +365,13 @@
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
+    </font>
+    <font>
+      <name val="Monospace"/>
+      <family val="0"/>
+      <color rgb="003F7F5F"/>
+      <sz val="10"/>
+      <u val="single"/>
     </font>
   </fonts>
   <fills count="7">
@@ -431,7 +544,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -550,6 +663,7 @@
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="14" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -610,7 +724,7 @@
       <rgbColor rgb="00666699"/>
       <rgbColor rgb="00969696"/>
       <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="003F7F5F"/>
       <rgbColor rgb="00003300"/>
       <rgbColor rgb="00333300"/>
       <rgbColor rgb="00993300"/>
@@ -629,18 +743,18 @@
   </sheetPr>
   <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A40" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
       <selection activeCell="R67" activeCellId="0" pane="topLeft" sqref="R67"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.15294117647059"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="10.0392156862745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.0862745098039"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.50980392156863"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.15294117647059"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.50980392156863"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.2"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="10.0941176470588"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.1372549019608"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.55686274509804"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.2"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.55686274509804"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -1614,15 +1728,15 @@
         <v>0</v>
       </c>
       <c r="E37" s="24" t="n">
-        <f aca="false">Sheet1!$B$30</f>
+        <f aca="false">ForwardKinematics!$B$30</f>
         <v>0</v>
       </c>
       <c r="F37" s="24" t="n">
-        <f aca="false">Sheet1!$C$30</f>
+        <f aca="false">ForwardKinematics!$C$30</f>
         <v>0</v>
       </c>
       <c r="G37" s="26" t="n">
-        <f aca="false">Sheet1!$D$30</f>
+        <f aca="false">ForwardKinematics!$D$30</f>
         <v>1</v>
       </c>
     </row>
@@ -1643,15 +1757,15 @@
         <v>-0.431724508025022</v>
       </c>
       <c r="E38" s="0" t="n">
-        <f aca="false">Sheet1!$B$31</f>
+        <f aca="false">ForwardKinematics!$B$31</f>
         <v>0.846615122810557</v>
       </c>
       <c r="F38" s="0" t="n">
-        <f aca="false">Sheet1!$C$31</f>
+        <f aca="false">ForwardKinematics!$C$31</f>
         <v>-0.532205631150654</v>
       </c>
       <c r="G38" s="7" t="n">
-        <f aca="false">Sheet1!$D$31</f>
+        <f aca="false">ForwardKinematics!$D$31</f>
         <v>0</v>
       </c>
     </row>
@@ -1672,15 +1786,15 @@
         <v>-0.000421846125105596</v>
       </c>
       <c r="E39" s="0" t="n">
-        <f aca="false">Sheet1!$B$32</f>
+        <f aca="false">ForwardKinematics!$B$32</f>
         <v>0.846615122810557</v>
       </c>
       <c r="F39" s="0" t="n">
-        <f aca="false">Sheet1!$C$32</f>
+        <f aca="false">ForwardKinematics!$C$32</f>
         <v>-0.532205631150654</v>
       </c>
       <c r="G39" s="7" t="n">
-        <f aca="false">Sheet1!$D$32</f>
+        <f aca="false">ForwardKinematics!$D$32</f>
         <v>0</v>
       </c>
     </row>
@@ -1701,15 +1815,15 @@
         <v>0</v>
       </c>
       <c r="E40" s="0" t="n">
-        <f aca="false">Sheet1!$B$33</f>
+        <f aca="false">ForwardKinematics!$B$33</f>
         <v>-0.0255360618110436</v>
       </c>
       <c r="F40" s="0" t="n">
-        <f aca="false">Sheet1!$C$33</f>
+        <f aca="false">ForwardKinematics!$C$33</f>
         <v>-0.0406219228825386</v>
       </c>
       <c r="G40" s="7" t="n">
-        <f aca="false">Sheet1!$D$33</f>
+        <f aca="false">ForwardKinematics!$D$33</f>
         <v>0.998848221167014</v>
       </c>
     </row>
@@ -1730,15 +1844,15 @@
         <v>0</v>
       </c>
       <c r="E41" s="0" t="n">
-        <f aca="false">Sheet1!$B$34</f>
+        <f aca="false">ForwardKinematics!$B$34</f>
         <v>0.99967366738032</v>
       </c>
       <c r="F41" s="0" t="n">
-        <f aca="false">Sheet1!$C$34</f>
+        <f aca="false">ForwardKinematics!$C$34</f>
         <v>-0.00172163968232636</v>
       </c>
       <c r="G41" s="7" t="n">
-        <f aca="false">Sheet1!$D$34</f>
+        <f aca="false">ForwardKinematics!$D$34</f>
         <v>0.0254871478040434</v>
       </c>
     </row>
@@ -1759,15 +1873,15 @@
         <v>0</v>
       </c>
       <c r="E42" s="12" t="n">
-        <f aca="false">Sheet1!$B$35</f>
+        <f aca="false">ForwardKinematics!$B$35</f>
         <v>-0.00172523895810973</v>
       </c>
       <c r="F42" s="12" t="n">
-        <f aca="false">Sheet1!$C$35</f>
+        <f aca="false">ForwardKinematics!$C$35</f>
         <v>-0.99999850466618</v>
       </c>
       <c r="G42" s="14" t="n">
-        <f aca="false">Sheet1!$D$35</f>
+        <f aca="false">ForwardKinematics!$D$35</f>
         <v>0.000119230621019983</v>
       </c>
     </row>
@@ -1814,27 +1928,27 @@
         <v>45</v>
       </c>
       <c r="B45" s="35" t="n">
-        <f aca="false">Sheet1!$B$37</f>
+        <f aca="false">ForwardKinematics!$B$37</f>
         <v>0.431742810234942</v>
       </c>
       <c r="C45" s="36" t="n">
-        <f aca="false">Sheet1!$B$38</f>
+        <f aca="false">ForwardKinematics!$B$38</f>
         <v>-0.219034126679394</v>
       </c>
       <c r="D45" s="36" t="n">
-        <f aca="false">Sheet1!$B$39</f>
+        <f aca="false">ForwardKinematics!$B$39</f>
         <v>-0.230060598169403</v>
       </c>
       <c r="E45" s="36" t="n">
-        <f aca="false">Sheet1!$B$40</f>
+        <f aca="false">ForwardKinematics!$B$40</f>
         <v>-0</v>
       </c>
       <c r="F45" s="36" t="n">
-        <f aca="false">Sheet1!$B$41</f>
+        <f aca="false">ForwardKinematics!$B$41</f>
         <v>-0</v>
       </c>
       <c r="G45" s="37" t="n">
-        <f aca="false">Sheet1!$B$42</f>
+        <f aca="false">ForwardKinematics!$B$42</f>
         <v>-0</v>
       </c>
       <c r="I45" s="38" t="n">
@@ -1848,27 +1962,27 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
       <c r="A46" s="34"/>
       <c r="B46" s="35" t="n">
-        <f aca="false">Sheet1!$C$37</f>
+        <f aca="false">ForwardKinematics!$C$37</f>
         <v>-0.12439649609166</v>
       </c>
       <c r="C46" s="36" t="n">
-        <f aca="false">Sheet1!$C$38</f>
+        <f aca="false">ForwardKinematics!$C$38</f>
         <v>-0.348432247245211</v>
       </c>
       <c r="D46" s="36" t="n">
-        <f aca="false">Sheet1!$C$39</f>
+        <f aca="false">ForwardKinematics!$C$39</f>
         <v>-0.365972793545891</v>
       </c>
       <c r="E46" s="36" t="n">
-        <f aca="false">Sheet1!$C$40</f>
+        <f aca="false">ForwardKinematics!$C$40</f>
         <v>0</v>
       </c>
       <c r="F46" s="36" t="n">
-        <f aca="false">Sheet1!$C$41</f>
+        <f aca="false">ForwardKinematics!$C$41</f>
         <v>0</v>
       </c>
       <c r="G46" s="37" t="n">
-        <f aca="false">Sheet1!$C$42</f>
+        <f aca="false">ForwardKinematics!$C$42</f>
         <v>0</v>
       </c>
       <c r="I46" s="38" t="n">
@@ -1882,27 +1996,27 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
       <c r="A47" s="34"/>
       <c r="B47" s="35" t="n">
-        <f aca="false">Sheet1!$D$37</f>
+        <f aca="false">ForwardKinematics!$D$37</f>
         <v>0</v>
       </c>
       <c r="C47" s="36" t="n">
-        <f aca="false">Sheet1!$D$38</f>
+        <f aca="false">ForwardKinematics!$D$38</f>
         <v>-0.431724508025022</v>
       </c>
       <c r="D47" s="36" t="n">
-        <f aca="false">Sheet1!$D$39</f>
+        <f aca="false">ForwardKinematics!$D$39</f>
         <v>-0.000421846125105596</v>
       </c>
       <c r="E47" s="36" t="n">
-        <f aca="false">Sheet1!$D$40</f>
+        <f aca="false">ForwardKinematics!$D$40</f>
         <v>0</v>
       </c>
       <c r="F47" s="36" t="n">
-        <f aca="false">Sheet1!$D$41</f>
+        <f aca="false">ForwardKinematics!$D$41</f>
         <v>0</v>
       </c>
       <c r="G47" s="37" t="n">
-        <f aca="false">Sheet1!$D$42</f>
+        <f aca="false">ForwardKinematics!$D$42</f>
         <v>0</v>
       </c>
       <c r="I47" s="38" t="n">
@@ -1918,27 +2032,27 @@
         <v>46</v>
       </c>
       <c r="B48" s="35" t="n">
-        <f aca="false">Sheet1!$E$37</f>
+        <f aca="false">ForwardKinematics!$E$37</f>
         <v>0</v>
       </c>
       <c r="C48" s="36" t="n">
-        <f aca="false">Sheet1!$E$38</f>
+        <f aca="false">ForwardKinematics!$E$38</f>
         <v>0.846615122810557</v>
       </c>
       <c r="D48" s="36" t="n">
-        <f aca="false">Sheet1!$E$39</f>
+        <f aca="false">ForwardKinematics!$E$39</f>
         <v>0.846615122810557</v>
       </c>
       <c r="E48" s="36" t="n">
-        <f aca="false">Sheet1!$E$40</f>
+        <f aca="false">ForwardKinematics!$E$40</f>
         <v>-0.0255360618110436</v>
       </c>
       <c r="F48" s="36" t="n">
-        <f aca="false">Sheet1!$E$41</f>
+        <f aca="false">ForwardKinematics!$E$41</f>
         <v>0.99967366738032</v>
       </c>
       <c r="G48" s="37" t="n">
-        <f aca="false">Sheet1!$E$42</f>
+        <f aca="false">ForwardKinematics!$E$42</f>
         <v>-0.00172523895810973</v>
       </c>
       <c r="I48" s="38" t="n">
@@ -1952,27 +2066,27 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
       <c r="A49" s="34"/>
       <c r="B49" s="35" t="n">
-        <f aca="false">Sheet1!$F$37</f>
+        <f aca="false">ForwardKinematics!$F$37</f>
         <v>0</v>
       </c>
       <c r="C49" s="36" t="n">
-        <f aca="false">Sheet1!$F$38</f>
+        <f aca="false">ForwardKinematics!$F$38</f>
         <v>-0.532205631150654</v>
       </c>
       <c r="D49" s="36" t="n">
-        <f aca="false">Sheet1!$F$39</f>
+        <f aca="false">ForwardKinematics!$F$39</f>
         <v>-0.532205631150654</v>
       </c>
       <c r="E49" s="36" t="n">
-        <f aca="false">Sheet1!$F$40</f>
+        <f aca="false">ForwardKinematics!$F$40</f>
         <v>-0.0406219228825386</v>
       </c>
       <c r="F49" s="36" t="n">
-        <f aca="false">Sheet1!$F$41</f>
+        <f aca="false">ForwardKinematics!$F$41</f>
         <v>-0.00172163968232636</v>
       </c>
       <c r="G49" s="37" t="n">
-        <f aca="false">Sheet1!$F$42</f>
+        <f aca="false">ForwardKinematics!$F$42</f>
         <v>-0.99999850466618</v>
       </c>
       <c r="I49" s="38" t="n">
@@ -1986,27 +2100,27 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50">
       <c r="A50" s="34"/>
       <c r="B50" s="40" t="n">
-        <f aca="false">Sheet1!$G$37</f>
+        <f aca="false">ForwardKinematics!$G$37</f>
         <v>1</v>
       </c>
       <c r="C50" s="41" t="n">
-        <f aca="false">Sheet1!$G$38</f>
+        <f aca="false">ForwardKinematics!$G$38</f>
         <v>0</v>
       </c>
       <c r="D50" s="41" t="n">
-        <f aca="false">Sheet1!$G$39</f>
+        <f aca="false">ForwardKinematics!$G$39</f>
         <v>0</v>
       </c>
       <c r="E50" s="41" t="n">
-        <f aca="false">Sheet1!$G$40</f>
+        <f aca="false">ForwardKinematics!$G$40</f>
         <v>0.998848221167014</v>
       </c>
       <c r="F50" s="41" t="n">
-        <f aca="false">Sheet1!$G$41</f>
+        <f aca="false">ForwardKinematics!$G$41</f>
         <v>0.0254871478040434</v>
       </c>
       <c r="G50" s="42" t="n">
-        <f aca="false">Sheet1!$G$42</f>
+        <f aca="false">ForwardKinematics!$G$42</f>
         <v>0.000119230621019983</v>
       </c>
       <c r="I50" s="38" t="n">
@@ -2028,61 +2142,61 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52">
       <c r="A52" s="43" t="str">
-        <f aca="false">Sheet1!$A$23</f>
+        <f aca="false">ForwardKinematics!$A$23</f>
         <v>01T</v>
       </c>
       <c r="B52" s="44" t="n">
-        <f aca="false">Sheet1!$B$23</f>
+        <f aca="false">ForwardKinematics!$B$23</f>
         <v>-0.532205631150654</v>
       </c>
       <c r="C52" s="44" t="n">
-        <f aca="false">Sheet1!$C$23</f>
+        <f aca="false">ForwardKinematics!$C$23</f>
         <v>0.846615122810557</v>
       </c>
       <c r="D52" s="44" t="n">
-        <f aca="false">Sheet1!$D$23</f>
+        <f aca="false">ForwardKinematics!$D$23</f>
         <v>0</v>
       </c>
       <c r="E52" s="45" t="n">
-        <f aca="false">Sheet1!$K$23</f>
+        <f aca="false">ForwardKinematics!$K$23</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="53">
       <c r="A53" s="43"/>
       <c r="B53" s="46" t="n">
-        <f aca="false">Sheet1!$E$23</f>
+        <f aca="false">ForwardKinematics!$E$23</f>
         <v>-0.846615122810557</v>
       </c>
       <c r="C53" s="46" t="n">
-        <f aca="false">Sheet1!$F$23</f>
+        <f aca="false">ForwardKinematics!$F$23</f>
         <v>-0.532205631150654</v>
       </c>
       <c r="D53" s="46" t="n">
-        <f aca="false">Sheet1!$G$23</f>
+        <f aca="false">ForwardKinematics!$G$23</f>
         <v>0</v>
       </c>
       <c r="E53" s="47" t="n">
-        <f aca="false">Sheet1!$L$23</f>
+        <f aca="false">ForwardKinematics!$L$23</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="54">
       <c r="A54" s="43"/>
       <c r="B54" s="48" t="n">
-        <f aca="false">Sheet1!$H$23</f>
+        <f aca="false">ForwardKinematics!$H$23</f>
         <v>0</v>
       </c>
       <c r="C54" s="48" t="n">
-        <f aca="false">Sheet1!$I$23</f>
+        <f aca="false">ForwardKinematics!$I$23</f>
         <v>0</v>
       </c>
       <c r="D54" s="48" t="n">
-        <f aca="false">Sheet1!$J$23</f>
+        <f aca="false">ForwardKinematics!$J$23</f>
         <v>1</v>
       </c>
       <c r="E54" s="47" t="n">
-        <f aca="false">Sheet1!$M$23</f>
+        <f aca="false">ForwardKinematics!$M$23</f>
         <v>0.674</v>
       </c>
     </row>
@@ -2103,61 +2217,61 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
       <c r="A56" s="43" t="str">
-        <f aca="false">Sheet1!$A$24</f>
+        <f aca="false">ForwardKinematics!$A$24</f>
         <v>02T</v>
       </c>
       <c r="B56" s="44" t="n">
-        <f aca="false">Sheet1!$B$24</f>
+        <f aca="false">ForwardKinematics!$B$24</f>
         <v>-0.531592647969898</v>
       </c>
       <c r="C56" s="44" t="n">
-        <f aca="false">Sheet1!$C$24</f>
+        <f aca="false">ForwardKinematics!$C$24</f>
         <v>0.846615122810557</v>
       </c>
       <c r="D56" s="44" t="n">
-        <f aca="false">Sheet1!$D$24</f>
+        <f aca="false">ForwardKinematics!$D$24</f>
         <v>-0.0255360618110436</v>
       </c>
       <c r="E56" s="45" t="n">
-        <f aca="false">Sheet1!$K$24</f>
+        <f aca="false">ForwardKinematics!$K$24</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="57">
       <c r="A57" s="43"/>
       <c r="B57" s="46" t="n">
-        <f aca="false">Sheet1!$E$24</f>
+        <f aca="false">ForwardKinematics!$E$24</f>
         <v>-0.845640009432418</v>
       </c>
       <c r="C57" s="46" t="n">
-        <f aca="false">Sheet1!$F$24</f>
+        <f aca="false">ForwardKinematics!$F$24</f>
         <v>-0.532205631150654</v>
       </c>
       <c r="D57" s="46" t="n">
-        <f aca="false">Sheet1!$G$24</f>
+        <f aca="false">ForwardKinematics!$G$24</f>
         <v>-0.0406219228825386</v>
       </c>
       <c r="E57" s="47" t="n">
-        <f aca="false">Sheet1!$L$24</f>
+        <f aca="false">ForwardKinematics!$L$24</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="58">
       <c r="A58" s="43"/>
       <c r="B58" s="48" t="n">
-        <f aca="false">Sheet1!$H$24</f>
+        <f aca="false">ForwardKinematics!$H$24</f>
         <v>-0.0479815701232499</v>
       </c>
       <c r="C58" s="48" t="n">
-        <f aca="false">Sheet1!$I$24</f>
+        <f aca="false">ForwardKinematics!$I$24</f>
         <v>0</v>
       </c>
       <c r="D58" s="48" t="n">
-        <f aca="false">Sheet1!$J$24</f>
+        <f aca="false">ForwardKinematics!$J$24</f>
         <v>0.998848221167014</v>
       </c>
       <c r="E58" s="47" t="n">
-        <f aca="false">Sheet1!$M$24</f>
+        <f aca="false">ForwardKinematics!$M$24</f>
         <v>0.674</v>
       </c>
     </row>
@@ -2178,61 +2292,61 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="60">
       <c r="A60" s="43" t="str">
-        <f aca="false">Sheet1!$A$25</f>
+        <f aca="false">ForwardKinematics!$A$25</f>
         <v>03T</v>
       </c>
       <c r="B60" s="44" t="n">
-        <f aca="false">Sheet1!$B$25</f>
+        <f aca="false">ForwardKinematics!$B$25</f>
         <v>-0.531592647969898</v>
       </c>
       <c r="C60" s="44" t="n">
-        <f aca="false">Sheet1!$C$25</f>
+        <f aca="false">ForwardKinematics!$C$25</f>
         <v>0.846615122810557</v>
       </c>
       <c r="D60" s="44" t="n">
-        <f aca="false">Sheet1!$D$25</f>
+        <f aca="false">ForwardKinematics!$D$25</f>
         <v>-0.0255360618110436</v>
       </c>
       <c r="E60" s="45" t="n">
-        <f aca="false">Sheet1!$K$25</f>
+        <f aca="false">ForwardKinematics!$K$25</f>
         <v>-0.1241719872084</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="61">
       <c r="A61" s="43"/>
       <c r="B61" s="46" t="n">
-        <f aca="false">Sheet1!$E$25</f>
+        <f aca="false">ForwardKinematics!$E$25</f>
         <v>-0.845640009432418</v>
       </c>
       <c r="C61" s="46" t="n">
-        <f aca="false">Sheet1!$F$25</f>
+        <f aca="false">ForwardKinematics!$F$25</f>
         <v>-0.532205631150654</v>
       </c>
       <c r="D61" s="46" t="n">
-        <f aca="false">Sheet1!$G$25</f>
+        <f aca="false">ForwardKinematics!$G$25</f>
         <v>-0.0406219228825386</v>
       </c>
       <c r="E61" s="47" t="n">
-        <f aca="false">Sheet1!$L$25</f>
+        <f aca="false">ForwardKinematics!$L$25</f>
         <v>-0.431385668925928</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="62">
       <c r="A62" s="43"/>
       <c r="B62" s="48" t="n">
-        <f aca="false">Sheet1!$H$25</f>
+        <f aca="false">ForwardKinematics!$H$25</f>
         <v>-0.0479815701232499</v>
       </c>
       <c r="C62" s="48" t="n">
-        <f aca="false">Sheet1!$I$25</f>
+        <f aca="false">ForwardKinematics!$I$25</f>
         <v>0</v>
       </c>
       <c r="D62" s="48" t="n">
-        <f aca="false">Sheet1!$J$25</f>
+        <f aca="false">ForwardKinematics!$J$25</f>
         <v>0.998848221167014</v>
       </c>
       <c r="E62" s="47" t="n">
-        <f aca="false">Sheet1!$M$25</f>
+        <f aca="false">ForwardKinematics!$M$25</f>
         <v>0.653281558020781</v>
       </c>
     </row>
@@ -2253,61 +2367,61 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="64">
       <c r="A64" s="43" t="str">
-        <f aca="false">Sheet1!$A$26</f>
+        <f aca="false">ForwardKinematics!$A$26</f>
         <v>04T</v>
       </c>
       <c r="B64" s="44" t="n">
-        <f aca="false">Sheet1!$B$26</f>
+        <f aca="false">ForwardKinematics!$B$26</f>
         <v>-0.000684319781590448</v>
       </c>
       <c r="C64" s="44" t="n">
-        <f aca="false">Sheet1!$C$26</f>
+        <f aca="false">ForwardKinematics!$C$26</f>
         <v>0.99967366738032</v>
       </c>
       <c r="D64" s="44" t="n">
-        <f aca="false">Sheet1!$D$26</f>
+        <f aca="false">ForwardKinematics!$D$26</f>
         <v>-0.0255360618110436</v>
       </c>
       <c r="E64" s="45" t="n">
-        <f aca="false">Sheet1!$K$26</f>
+        <f aca="false">ForwardKinematics!$K$26</f>
         <v>-0.12439649609166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="65">
       <c r="A65" s="43"/>
       <c r="B65" s="46" t="n">
-        <f aca="false">Sheet1!$E$26</f>
+        <f aca="false">ForwardKinematics!$E$26</f>
         <v>-0.999173105792049</v>
       </c>
       <c r="C65" s="46" t="n">
-        <f aca="false">Sheet1!$F$26</f>
+        <f aca="false">ForwardKinematics!$F$26</f>
         <v>-0.00172163968232636</v>
       </c>
       <c r="D65" s="46" t="n">
-        <f aca="false">Sheet1!$G$26</f>
+        <f aca="false">ForwardKinematics!$G$26</f>
         <v>-0.0406219228825386</v>
       </c>
       <c r="E65" s="47" t="n">
-        <f aca="false">Sheet1!$L$26</f>
+        <f aca="false">ForwardKinematics!$L$26</f>
         <v>-0.431742810234942</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="66">
       <c r="A66" s="43"/>
       <c r="B66" s="48" t="n">
-        <f aca="false">Sheet1!$H$26</f>
+        <f aca="false">ForwardKinematics!$H$26</f>
         <v>-0.0406526305213721</v>
       </c>
       <c r="C66" s="48" t="n">
-        <f aca="false">Sheet1!$I$26</f>
+        <f aca="false">ForwardKinematics!$I$26</f>
         <v>0.0254871478040434</v>
       </c>
       <c r="D66" s="48" t="n">
-        <f aca="false">Sheet1!$J$26</f>
+        <f aca="false">ForwardKinematics!$J$26</f>
         <v>0.998848221167014</v>
       </c>
       <c r="E66" s="47" t="n">
-        <f aca="false">Sheet1!$M$26</f>
+        <f aca="false">ForwardKinematics!$M$26</f>
         <v>1.0855592054256</v>
       </c>
     </row>
@@ -2328,61 +2442,61 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="68">
       <c r="A68" s="43" t="str">
-        <f aca="false">Sheet1!$A$27</f>
+        <f aca="false">ForwardKinematics!$A$27</f>
         <v>05T</v>
       </c>
       <c r="B68" s="44" t="n">
-        <f aca="false">Sheet1!$B$27</f>
+        <f aca="false">ForwardKinematics!$B$27</f>
         <v>0.0254869044200808</v>
       </c>
       <c r="C68" s="44" t="n">
-        <f aca="false">Sheet1!$C$27</f>
+        <f aca="false">ForwardKinematics!$C$27</f>
         <v>0.99967366738032</v>
       </c>
       <c r="D68" s="44" t="n">
-        <f aca="false">Sheet1!$D$27</f>
+        <f aca="false">ForwardKinematics!$D$27</f>
         <v>-0.00172523895810973</v>
       </c>
       <c r="E68" s="45" t="n">
-        <f aca="false">Sheet1!$K$27</f>
+        <f aca="false">ForwardKinematics!$K$27</f>
         <v>-0.12439649609166</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="69">
       <c r="A69" s="43"/>
       <c r="B69" s="46" t="n">
-        <f aca="false">Sheet1!$E$27</f>
+        <f aca="false">ForwardKinematics!$E$27</f>
         <v>-0.000163163132501712</v>
       </c>
       <c r="C69" s="46" t="n">
-        <f aca="false">Sheet1!$F$27</f>
+        <f aca="false">ForwardKinematics!$F$27</f>
         <v>-0.00172163968232636</v>
       </c>
       <c r="D69" s="46" t="n">
-        <f aca="false">Sheet1!$G$27</f>
+        <f aca="false">ForwardKinematics!$G$27</f>
         <v>-0.99999850466618</v>
       </c>
       <c r="E69" s="47" t="n">
-        <f aca="false">Sheet1!$L$27</f>
+        <f aca="false">ForwardKinematics!$L$27</f>
         <v>-0.431742810234942</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="70">
       <c r="A70" s="43"/>
       <c r="B70" s="48" t="n">
-        <f aca="false">Sheet1!$H$27</f>
+        <f aca="false">ForwardKinematics!$H$27</f>
         <v>-0.999675142774328</v>
       </c>
       <c r="C70" s="48" t="n">
-        <f aca="false">Sheet1!$I$27</f>
+        <f aca="false">ForwardKinematics!$I$27</f>
         <v>0.0254871478040434</v>
       </c>
       <c r="D70" s="48" t="n">
-        <f aca="false">Sheet1!$J$27</f>
+        <f aca="false">ForwardKinematics!$J$27</f>
         <v>0.000119230621019983</v>
       </c>
       <c r="E70" s="47" t="n">
-        <f aca="false">Sheet1!$M$27</f>
+        <f aca="false">ForwardKinematics!$M$27</f>
         <v>1.0855592054256</v>
       </c>
     </row>
@@ -2407,23 +2521,23 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="72">
       <c r="A72" s="43" t="str">
-        <f aca="false">Sheet1!$A$28</f>
+        <f aca="false">ForwardKinematics!$A$28</f>
         <v>06T</v>
       </c>
       <c r="B72" s="44" t="n">
-        <f aca="false">Sheet1!$B$28</f>
+        <f aca="false">ForwardKinematics!$B$28</f>
         <v>0.000102950959787951</v>
       </c>
       <c r="C72" s="44" t="n">
-        <f aca="false">Sheet1!$C$28</f>
+        <f aca="false">ForwardKinematics!$C$28</f>
         <v>-0.999998506474703</v>
       </c>
       <c r="D72" s="44" t="n">
-        <f aca="false">Sheet1!$D$28</f>
+        <f aca="false">ForwardKinematics!$D$28</f>
         <v>-0.00172523895810973</v>
       </c>
       <c r="E72" s="45" t="n">
-        <f aca="false">Sheet1!$K$28</f>
+        <f aca="false">ForwardKinematics!$K$28</f>
         <v>-0.12439649609166</v>
       </c>
       <c r="I72" s="51" t="s">
@@ -2437,19 +2551,19 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="73">
       <c r="A73" s="43"/>
       <c r="B73" s="46" t="n">
-        <f aca="false">Sheet1!$E$28</f>
+        <f aca="false">ForwardKinematics!$E$28</f>
         <v>0.000119053182560803</v>
       </c>
       <c r="C73" s="46" t="n">
-        <f aca="false">Sheet1!$F$28</f>
+        <f aca="false">ForwardKinematics!$F$28</f>
         <v>0.00172525121164737</v>
       </c>
       <c r="D73" s="46" t="n">
-        <f aca="false">Sheet1!$G$28</f>
+        <f aca="false">ForwardKinematics!$G$28</f>
         <v>-0.99999850466618</v>
       </c>
       <c r="E73" s="47" t="n">
-        <f aca="false">Sheet1!$L$28</f>
+        <f aca="false">ForwardKinematics!$L$28</f>
         <v>-0.431742810234942</v>
       </c>
       <c r="I73" s="52" t="s">
@@ -2463,19 +2577,19 @@
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="74">
       <c r="A74" s="43"/>
       <c r="B74" s="48" t="n">
-        <f aca="false">Sheet1!$H$28</f>
+        <f aca="false">ForwardKinematics!$H$28</f>
         <v>0.99999998761372</v>
       </c>
       <c r="C74" s="48" t="n">
-        <f aca="false">Sheet1!$I$28</f>
+        <f aca="false">ForwardKinematics!$I$28</f>
         <v>0.000102745410653259</v>
       </c>
       <c r="D74" s="48" t="n">
-        <f aca="false">Sheet1!$J$28</f>
+        <f aca="false">ForwardKinematics!$J$28</f>
         <v>0.000119230621019983</v>
       </c>
       <c r="E74" s="47" t="n">
-        <f aca="false">Sheet1!$M$28</f>
+        <f aca="false">ForwardKinematics!$M$28</f>
         <v>1.0855592054256</v>
       </c>
       <c r="I74" s="52" t="s">
@@ -2699,4 +2813,116 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A17"/>
+  <sheetViews>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
+      <selection activeCell="D8" activeCellId="0" pane="topLeft" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.5607843137255"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5764705882353"/>
+  </cols>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="1">
+      <c r="A1" s="62" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
+      <c r="A2" s="62" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="3">
+      <c r="A3" s="62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="4">
+      <c r="A4" s="62" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
+      <c r="A5" s="62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="6">
+      <c r="A6" s="62" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
+      <c r="A7" s="62" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
+      <c r="A8" s="62" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
+      <c r="A9" s="62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
+      <c r="A10" s="62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
+      <c r="A11" s="62" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
+      <c r="A12" s="62" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
+      <c r="A13" s="62" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
+      <c r="A14" s="62" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="15">
+      <c r="A15" s="62" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+      <c r="A16" s="62" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+      <c r="A17" s="62" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added image of puma560 kinematics for clarity
</commit_message>
<xml_diff>
--- a/constrained_ik/test/puma_560_jacobian.xlsx
+++ b/constrained_ik/test/puma_560_jacobian.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="176" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="176" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="ForwardKinematics" sheetId="1" state="visible" r:id="rId2"/>
@@ -222,6 +222,7 @@
     <r>
       <rPr>
         <rFont val="Monospace"/>
+        <charset val="1"/>
         <family val="0"/>
         <color rgb="003F7F5F"/>
         <sz val="10"/>
@@ -232,6 +233,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <sz val="10"/>
       </rPr>
@@ -248,6 +250,7 @@
     <r>
       <rPr>
         <rFont val="Monospace"/>
+        <charset val="1"/>
         <family val="0"/>
         <color rgb="003F7F5F"/>
         <sz val="10"/>
@@ -258,6 +261,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <sz val="10"/>
       </rPr>
@@ -271,6 +275,7 @@
     <r>
       <rPr>
         <rFont val="Monospace"/>
+        <charset val="1"/>
         <family val="0"/>
         <color rgb="003F7F5F"/>
         <sz val="10"/>
@@ -281,6 +286,7 @@
     <r>
       <rPr>
         <rFont val="Arial"/>
+        <charset val="1"/>
         <family val="2"/>
         <sz val="10"/>
       </rPr>
@@ -319,16 +325,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="0.00" numFmtId="165"/>
-    <numFmt formatCode="0.00000" numFmtId="166"/>
-    <numFmt formatCode="0.0000" numFmtId="167"/>
-    <numFmt formatCode="0" numFmtId="168"/>
+    <numFmt formatCode="0.######" numFmtId="166"/>
+    <numFmt formatCode="0.00000" numFmtId="167"/>
+    <numFmt formatCode="0.0000" numFmtId="168"/>
+    <numFmt formatCode="0" numFmtId="169"/>
   </numFmts>
   <fonts count="7">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -349,6 +357,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <color rgb="00FFFF00"/>
@@ -356,12 +365,14 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Monospace"/>
+      <charset val="1"/>
       <family val="0"/>
       <color rgb="003F7F5F"/>
       <sz val="10"/>
@@ -538,7 +549,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="72">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -577,11 +588,17 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="3" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="4" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="7" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="10" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
@@ -600,36 +617,36 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="167" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="6" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="4" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="166" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="166" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="4" fontId="0" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="167" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="4" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="10" fillId="4" fontId="0" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="10" fillId="4" fontId="0" numFmtId="168" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="11" fillId="4" fontId="0" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="11" fillId="4" fontId="0" numFmtId="168" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="168" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="168" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="167" xfId="0">
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="4" fontId="0" numFmtId="168" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="168" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="169" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="168" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="169" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -657,6 +674,9 @@
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="14" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="3" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="5" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="false" applyProtection="false" borderId="6" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
@@ -730,6 +750,47 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>34560</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>92880</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>93240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr descr="" id="0" name="Graphics 1"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5321520" y="0"/>
+          <a:ext cx="4984560" cy="7928280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -737,18 +798,18 @@
   </sheetPr>
   <dimension ref="A1:M89"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="B28" activeCellId="0" pane="topLeft" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.24313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="10.1372549019608"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.1843137254902"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.6"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.24313725490196"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.6"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.29019607843137"/>
+    <col collapsed="false" hidden="false" max="6" min="2" style="0" width="10.1843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.2392156862745"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.29019607843137"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="8.64705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -785,15 +846,14 @@
         <v>3</v>
       </c>
       <c r="B3" s="5" t="n">
-        <f aca="false">-PI()/2</f>
-        <v>-1.5707963267949</v>
+        <v>0</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>-3.93</v>
       </c>
       <c r="D3" s="6" t="n">
         <f aca="false">(B3-C3)/(E3-C3)</f>
-        <v>0.499831286695996</v>
+        <v>0.832627118644068</v>
       </c>
       <c r="E3" s="7" t="n">
         <v>0.79</v>
@@ -939,14 +999,14 @@
       </c>
       <c r="B10" s="5" t="n">
         <f aca="false">COS(B3)</f>
-        <v>6.12323399573677E-017</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="D10" s="5" t="n">
         <f aca="false">SIN(B3)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="5" t="n">
         <v>0</v>
@@ -959,14 +1019,14 @@
       </c>
       <c r="H10" s="5" t="n">
         <f aca="false">-SIN(B3)</f>
-        <v>1</v>
+        <v>-0</v>
       </c>
       <c r="I10" s="5" t="n">
         <v>0</v>
       </c>
       <c r="J10" s="19" t="n">
         <f aca="false">COS(B3)</f>
-        <v>6.12323399573677E-017</v>
+        <v>1</v>
       </c>
       <c r="K10" s="20" t="n">
         <v>0</v>
@@ -1324,51 +1384,51 @@
       <c r="A24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="27" t="n">
         <f aca="false">B23*$B10+C23*$E10+D23*$H10</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" s="27" t="n">
         <f aca="false">B23*$C10+C23*$F10+D23*$I10</f>
         <v>0</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="27" t="n">
         <f aca="false">B23*$D10+C23*$G10+D23*$J10</f>
-        <v>-1</v>
-      </c>
-      <c r="E24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="27" t="n">
         <f aca="false">E23*$B10+F23*$E10+G23*$H10</f>
         <v>0</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="27" t="n">
         <f aca="false">E23*$C10+F23*$F10+G23*$I10</f>
         <v>1</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="27" t="n">
         <f aca="false">E23*$D10+F23*$G10+G23*$J10</f>
         <v>0</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="27" t="n">
         <f aca="false">H23*$B10+I23*$E10+J23*$H10</f>
-        <v>1</v>
-      </c>
-      <c r="I24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" s="27" t="n">
         <f aca="false">H23*$C10+I23*$F10+J23*$I10</f>
         <v>0</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="J24" s="27" t="n">
         <f aca="false">H23*$D10+I23*$G10+J23*$J10</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="K24" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K24" s="28" t="n">
         <f aca="false">B23*$K10+C23*$L10+D23*$M10+K23</f>
         <v>0</v>
       </c>
-      <c r="L24" s="0" t="n">
+      <c r="L24" s="27" t="n">
         <f aca="false">E23*$K10+F23*$L10+G23*$M10+L23</f>
         <v>0</v>
       </c>
-      <c r="M24" s="7" t="n">
+      <c r="M24" s="29" t="n">
         <f aca="false">H23*$K10+I23*$L10+J23*$M10+M23</f>
         <v>0.674</v>
       </c>
@@ -1377,212 +1437,212 @@
       <c r="A25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="27" t="n">
         <f aca="false">B24*$B11+C24*$E11+D24*$H11</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" s="27" t="n">
         <f aca="false">B24*$C11+C24*$F11+D24*$I11</f>
         <v>0</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="27" t="n">
         <f aca="false">B24*$D11+C24*$G11+D24*$J11</f>
-        <v>-1</v>
-      </c>
-      <c r="E25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" s="27" t="n">
         <f aca="false">E24*$B11+F24*$E11+G24*$H11</f>
         <v>0</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="27" t="n">
         <f aca="false">E24*$C11+F24*$F11+G24*$I11</f>
         <v>1</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="27" t="n">
         <f aca="false">E24*$D11+F24*$G11+G24*$J11</f>
         <v>0</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="27" t="n">
         <f aca="false">H24*$B11+I24*$E11+J24*$H11</f>
-        <v>1</v>
-      </c>
-      <c r="I25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" s="27" t="n">
         <f aca="false">H24*$C11+I24*$F11+J24*$I11</f>
         <v>0</v>
       </c>
-      <c r="J25" s="0" t="n">
+      <c r="J25" s="27" t="n">
         <f aca="false">H24*$D11+I24*$G11+J24*$J11</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="K25" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="28" t="n">
         <f aca="false">B24*$K11+C24*$L11+D24*$M11+K24</f>
-        <v>2.64401243935914E-017</v>
-      </c>
-      <c r="L25" s="0" t="n">
+        <v>0.4318</v>
+      </c>
+      <c r="L25" s="27" t="n">
         <f aca="false">E24*$K11+F24*$L11+G24*$M11+L24</f>
         <v>0.12446</v>
       </c>
-      <c r="M25" s="7" t="n">
+      <c r="M25" s="29" t="n">
         <f aca="false">H24*$K11+I24*$L11+J24*$M11+M24</f>
-        <v>1.1058</v>
+        <v>0.674</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
       <c r="A26" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="27" t="n">
         <f aca="false">B25*$B12+C25*$E12+D25*$H12</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" s="27" t="n">
         <f aca="false">B25*$C12+C25*$F12+D25*$I12</f>
         <v>0</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="27" t="n">
         <f aca="false">B25*$D12+C25*$G12+D25*$J12</f>
-        <v>-1</v>
-      </c>
-      <c r="E26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" s="27" t="n">
         <f aca="false">E25*$B12+F25*$E12+G25*$H12</f>
         <v>0</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="27" t="n">
         <f aca="false">E25*$C12+F25*$F12+G25*$I12</f>
         <v>1</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="27" t="n">
         <f aca="false">E25*$D12+F25*$G12+G25*$J12</f>
         <v>0</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="27" t="n">
         <f aca="false">H25*$B12+I25*$E12+J25*$H12</f>
-        <v>1</v>
-      </c>
-      <c r="I26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="27" t="n">
         <f aca="false">H25*$C12+I25*$F12+J25*$I12</f>
         <v>0</v>
       </c>
-      <c r="J26" s="0" t="n">
+      <c r="J26" s="27" t="n">
         <f aca="false">H25*$D12+I25*$G12+J25*$J12</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="K26" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" s="28" t="n">
         <f aca="false">B25*$K12+C25*$L12+D25*$M12+K25</f>
-        <v>-0.4318</v>
-      </c>
-      <c r="L26" s="0" t="n">
+        <v>0.41148</v>
+      </c>
+      <c r="L26" s="27" t="n">
         <f aca="false">E25*$K12+F25*$L12+G25*$M12+L25</f>
         <v>0.12446</v>
       </c>
-      <c r="M26" s="7" t="n">
+      <c r="M26" s="29" t="n">
         <f aca="false">H25*$K12+I25*$L12+J25*$M12+M25</f>
-        <v>1.08548</v>
+        <v>1.1058</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="27" t="n">
         <f aca="false">B26*$B13+C26*$E13+D26*$H13</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C27" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="27" t="n">
         <f aca="false">B26*$C13+C26*$F13+D26*$I13</f>
         <v>0</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="27" t="n">
         <f aca="false">B26*$D13+C26*$G13+D26*$J13</f>
-        <v>-1</v>
-      </c>
-      <c r="E27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="27" t="n">
         <f aca="false">E26*$B13+F26*$E13+G26*$H13</f>
         <v>0</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="27" t="n">
         <f aca="false">E26*$C13+F26*$F13+G26*$I13</f>
         <v>1</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="27" t="n">
         <f aca="false">E26*$D13+F26*$G13+G26*$J13</f>
         <v>0</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="27" t="n">
         <f aca="false">H26*$B13+I26*$E13+J26*$H13</f>
-        <v>1</v>
-      </c>
-      <c r="I27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="27" t="n">
         <f aca="false">H26*$C13+I26*$F13+J26*$I13</f>
         <v>0</v>
       </c>
-      <c r="J27" s="0" t="n">
+      <c r="J27" s="27" t="n">
         <f aca="false">H26*$D13+I26*$G13+J26*$J13</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="K27" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K27" s="28" t="n">
         <f aca="false">B26*$K13+C26*$L13+D26*$M13+K26</f>
-        <v>-0.4318</v>
-      </c>
-      <c r="L27" s="0" t="n">
+        <v>0.41148</v>
+      </c>
+      <c r="L27" s="27" t="n">
         <f aca="false">E26*$K13+F26*$L13+G26*$M13+L26</f>
         <v>0.12446</v>
       </c>
-      <c r="M27" s="7" t="n">
+      <c r="M27" s="29" t="n">
         <f aca="false">H26*$K13+I26*$L13+J26*$M13+M26</f>
-        <v>1.08548</v>
+        <v>1.1058</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="12" t="n">
+      <c r="B28" s="30" t="n">
         <f aca="false">B27*$B14+C27*$E14+D27*$H14</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C28" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" s="30" t="n">
         <f aca="false">B27*$C14+C27*$F14+D27*$I14</f>
         <v>0</v>
       </c>
-      <c r="D28" s="12" t="n">
+      <c r="D28" s="30" t="n">
         <f aca="false">B27*$D14+C27*$G14+D27*$J14</f>
-        <v>-1</v>
-      </c>
-      <c r="E28" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" s="30" t="n">
         <f aca="false">E27*$B14+F27*$E14+G27*$H14</f>
         <v>0</v>
       </c>
-      <c r="F28" s="12" t="n">
+      <c r="F28" s="30" t="n">
         <f aca="false">E27*$C14+F27*$F14+G27*$I14</f>
         <v>1</v>
       </c>
-      <c r="G28" s="12" t="n">
+      <c r="G28" s="30" t="n">
         <f aca="false">E27*$D14+F27*$G14+G27*$J14</f>
         <v>0</v>
       </c>
-      <c r="H28" s="12" t="n">
+      <c r="H28" s="30" t="n">
         <f aca="false">H27*$B14+I27*$E14+J27*$H14</f>
-        <v>1</v>
-      </c>
-      <c r="I28" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="30" t="n">
         <f aca="false">H27*$C14+I27*$F14+J27*$I14</f>
         <v>0</v>
       </c>
-      <c r="J28" s="12" t="n">
+      <c r="J28" s="30" t="n">
         <f aca="false">H27*$D14+I27*$G14+J27*$J14</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="K28" s="28" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" s="31" t="n">
         <f aca="false">B27*$K14+C27*$L14+D27*$M14+K27</f>
-        <v>-0.4318</v>
-      </c>
-      <c r="L28" s="12" t="n">
+        <v>0.41148</v>
+      </c>
+      <c r="L28" s="30" t="n">
         <f aca="false">E27*$K14+F27*$L14+G27*$M14+L27</f>
         <v>0.12446</v>
       </c>
-      <c r="M28" s="14" t="n">
+      <c r="M28" s="32" t="n">
         <f aca="false">H27*$K14+I27*$L14+J27*$M14+M27</f>
-        <v>1.08548</v>
+        <v>1.1058</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="29">
@@ -1597,15 +1657,15 @@
       <c r="A30" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="24" t="n">
+      <c r="B30" s="33" t="n">
         <f aca="false">B23*$B16+C23*$C16+D23*$D16</f>
         <v>0</v>
       </c>
-      <c r="C30" s="24" t="n">
+      <c r="C30" s="33" t="n">
         <f aca="false">E23*$B16+F23*$C16+G23*$D16</f>
         <v>0</v>
       </c>
-      <c r="D30" s="26" t="n">
+      <c r="D30" s="34" t="n">
         <f aca="false">H23*$B16+I23*$C16+J23*$D16</f>
         <v>1</v>
       </c>
@@ -1650,7 +1710,7 @@
       </c>
       <c r="B33" s="0" t="n">
         <f aca="false">B26*$B19+C26*$C19+D26*$D19</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C33" s="0" t="n">
         <f aca="false">E26*$B19+F26*$C19+G26*$D19</f>
@@ -1658,7 +1718,7 @@
       </c>
       <c r="D33" s="7" t="n">
         <f aca="false">H26*$B19+I26*$C19+J26*$D19</f>
-        <v>6.12323399573677E-017</v>
+        <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
@@ -1684,7 +1744,7 @@
       </c>
       <c r="B35" s="12" t="n">
         <f aca="false">B28*$B21+C28*$C21+D28*$D21</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C35" s="12" t="n">
         <f aca="false">E28*$B21+F28*$C21+G28*$D21</f>
@@ -1692,7 +1752,7 @@
       </c>
       <c r="D35" s="14" t="n">
         <f aca="false">H28*$B21+I28*$C21+J28*$D21</f>
-        <v>6.12323399573677E-017</v>
+        <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
@@ -1710,27 +1770,27 @@
       <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="24" t="n">
+      <c r="B37" s="33" t="n">
         <f aca="false">$F37*($M$28-$M23)-$G37*($L$28-$L23)</f>
         <v>-0.12446</v>
       </c>
-      <c r="C37" s="24" t="n">
+      <c r="C37" s="33" t="n">
         <f aca="false">-$E37*($M$28-$M23)+$G37*($K$28-$K23)</f>
-        <v>-0.4318</v>
-      </c>
-      <c r="D37" s="24" t="n">
+        <v>0.41148</v>
+      </c>
+      <c r="D37" s="33" t="n">
         <f aca="false">$E37*($L$28-$L23)-$F37*($K$28-$K23)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="24" t="n">
+      <c r="E37" s="33" t="n">
         <f aca="false">ForwardKinematics!$B$30</f>
         <v>0</v>
       </c>
-      <c r="F37" s="24" t="n">
+      <c r="F37" s="33" t="n">
         <f aca="false">ForwardKinematics!$C$30</f>
         <v>0</v>
       </c>
-      <c r="G37" s="26" t="n">
+      <c r="G37" s="34" t="n">
         <f aca="false">ForwardKinematics!$D$30</f>
         <v>1</v>
       </c>
@@ -1741,15 +1801,15 @@
       </c>
       <c r="B38" s="0" t="n">
         <f aca="false">$F38*($M$28-$M24)-$G38*($L$28-$L24)</f>
-        <v>0.41148</v>
+        <v>0.4318</v>
       </c>
       <c r="C38" s="0" t="n">
         <f aca="false">-$E38*($M$28-$M24)+$G38*($K$28-$K24)</f>
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D38" s="0" t="n">
         <f aca="false">$E38*($L$28-$L24)-$F38*($K$28-$K24)</f>
-        <v>0.4318</v>
+        <v>-0.41148</v>
       </c>
       <c r="E38" s="0" t="n">
         <f aca="false">ForwardKinematics!$B$31</f>
@@ -1770,15 +1830,15 @@
       </c>
       <c r="B39" s="0" t="n">
         <f aca="false">$F39*($M$28-$M25)-$G39*($L$28-$L25)</f>
-        <v>-0.0203199999999999</v>
+        <v>0.4318</v>
       </c>
       <c r="C39" s="0" t="n">
         <f aca="false">-$E39*($M$28-$M25)+$G39*($K$28-$K25)</f>
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D39" s="0" t="n">
         <f aca="false">$E39*($L$28-$L25)-$F39*($K$28-$K25)</f>
-        <v>0.4318</v>
+        <v>0.02032</v>
       </c>
       <c r="E39" s="0" t="n">
         <f aca="false">ForwardKinematics!$B$32</f>
@@ -1807,11 +1867,11 @@
       </c>
       <c r="D40" s="0" t="n">
         <f aca="false">$E40*($L$28-$L26)-$F40*($K$28-$K26)</f>
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E40" s="0" t="n">
         <f aca="false">ForwardKinematics!$B$33</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F40" s="0" t="n">
         <f aca="false">ForwardKinematics!$C$33</f>
@@ -1819,7 +1879,7 @@
       </c>
       <c r="G40" s="7" t="n">
         <f aca="false">ForwardKinematics!$D$33</f>
-        <v>6.12323399573677E-017</v>
+        <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="41">
@@ -1865,11 +1925,11 @@
       </c>
       <c r="D42" s="12" t="n">
         <f aca="false">$E42*($L$28-$L28)-$F42*($K$28-$K28)</f>
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="E42" s="12" t="n">
         <f aca="false">ForwardKinematics!$B$35</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F42" s="12" t="n">
         <f aca="false">ForwardKinematics!$C$35</f>
@@ -1877,7 +1937,7 @@
       </c>
       <c r="G42" s="14" t="n">
         <f aca="false">ForwardKinematics!$D$35</f>
-        <v>6.12323399573677E-017</v>
+        <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="43">
@@ -1889,239 +1949,239 @@
       <c r="E43" s="15"/>
       <c r="F43" s="15"/>
       <c r="G43" s="15"/>
-      <c r="I43" s="29" t="s">
+      <c r="I43" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="J43" s="30" t="s">
+      <c r="J43" s="36" t="s">
         <v>44</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="44">
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="32" t="s">
+      <c r="C44" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="32" t="s">
+      <c r="D44" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="E44" s="32" t="s">
+      <c r="E44" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="F44" s="32" t="s">
+      <c r="F44" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="G44" s="33" t="s">
+      <c r="G44" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="I44" s="29"/>
-      <c r="J44" s="29"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="45">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="B45" s="35" t="n">
+      <c r="B45" s="41" t="n">
         <f aca="false">ForwardKinematics!$B$37</f>
         <v>-0.12446</v>
       </c>
-      <c r="C45" s="36" t="n">
+      <c r="C45" s="42" t="n">
         <f aca="false">ForwardKinematics!$B$38</f>
+        <v>0.4318</v>
+      </c>
+      <c r="D45" s="42" t="n">
+        <f aca="false">ForwardKinematics!$B$39</f>
+        <v>0.4318</v>
+      </c>
+      <c r="E45" s="42" t="n">
+        <f aca="false">ForwardKinematics!$B$40</f>
+        <v>0</v>
+      </c>
+      <c r="F45" s="42" t="n">
+        <f aca="false">ForwardKinematics!$B$41</f>
+        <v>0</v>
+      </c>
+      <c r="G45" s="43" t="n">
+        <f aca="false">ForwardKinematics!$B$42</f>
+        <v>0</v>
+      </c>
+      <c r="I45" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" s="45" t="n">
+        <f aca="false">B45*$I$45+C45*$I$46+D45*$I$47+E45*$I$48+F45*$I$49+G45*$I$50</f>
+        <v>0.4318</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
+      <c r="A46" s="40"/>
+      <c r="B46" s="41" t="n">
+        <f aca="false">ForwardKinematics!$C$37</f>
         <v>0.41148</v>
       </c>
-      <c r="D45" s="36" t="n">
-        <f aca="false">ForwardKinematics!$B$39</f>
-        <v>-0.0203199999999999</v>
-      </c>
-      <c r="E45" s="36" t="n">
-        <f aca="false">ForwardKinematics!$B$40</f>
-        <v>0</v>
-      </c>
-      <c r="F45" s="36" t="n">
-        <f aca="false">ForwardKinematics!$B$41</f>
-        <v>0</v>
-      </c>
-      <c r="G45" s="37" t="n">
-        <f aca="false">ForwardKinematics!$B$42</f>
-        <v>0</v>
-      </c>
-      <c r="I45" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J45" s="39" t="n">
-        <f aca="false">B45*$I$45+C45*$I$46+D45*$I$47+E45*$I$48+F45*$I$49+G45*$I$50</f>
-        <v>-0.0203199999999999</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="46">
-      <c r="A46" s="34"/>
-      <c r="B46" s="35" t="n">
-        <f aca="false">ForwardKinematics!$C$37</f>
-        <v>-0.4318</v>
-      </c>
-      <c r="C46" s="36" t="n">
+      <c r="C46" s="42" t="n">
         <f aca="false">ForwardKinematics!$C$38</f>
+        <v>0</v>
+      </c>
+      <c r="D46" s="42" t="n">
+        <f aca="false">ForwardKinematics!$C$39</f>
         <v>-0</v>
       </c>
-      <c r="D46" s="36" t="n">
-        <f aca="false">ForwardKinematics!$C$39</f>
-        <v>0</v>
-      </c>
-      <c r="E46" s="36" t="n">
+      <c r="E46" s="42" t="n">
         <f aca="false">ForwardKinematics!$C$40</f>
         <v>0</v>
       </c>
-      <c r="F46" s="36" t="n">
+      <c r="F46" s="42" t="n">
         <f aca="false">ForwardKinematics!$C$41</f>
         <v>0</v>
       </c>
-      <c r="G46" s="37" t="n">
+      <c r="G46" s="43" t="n">
         <f aca="false">ForwardKinematics!$C$42</f>
         <v>0</v>
       </c>
-      <c r="I46" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J46" s="39" t="n">
+      <c r="I46" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J46" s="45" t="n">
         <f aca="false">B46*$I$45+C46*$I$46+D46*$I$47+E46*$I$48+F46*$I$49+G46*$I$50</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="47">
-      <c r="A47" s="34"/>
-      <c r="B47" s="35" t="n">
+      <c r="A47" s="40"/>
+      <c r="B47" s="41" t="n">
         <f aca="false">ForwardKinematics!$D$37</f>
         <v>0</v>
       </c>
-      <c r="C47" s="36" t="n">
+      <c r="C47" s="42" t="n">
         <f aca="false">ForwardKinematics!$D$38</f>
-        <v>0.4318</v>
-      </c>
-      <c r="D47" s="36" t="n">
+        <v>-0.41148</v>
+      </c>
+      <c r="D47" s="42" t="n">
         <f aca="false">ForwardKinematics!$D$39</f>
-        <v>0.4318</v>
-      </c>
-      <c r="E47" s="36" t="n">
+        <v>0.02032</v>
+      </c>
+      <c r="E47" s="42" t="n">
         <f aca="false">ForwardKinematics!$D$40</f>
-        <v>-0</v>
-      </c>
-      <c r="F47" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" s="42" t="n">
         <f aca="false">ForwardKinematics!$D$41</f>
         <v>0</v>
       </c>
-      <c r="G47" s="37" t="n">
+      <c r="G47" s="43" t="n">
         <f aca="false">ForwardKinematics!$D$42</f>
-        <v>-0</v>
-      </c>
-      <c r="I47" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="J47" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="J47" s="45" t="n">
         <f aca="false">B47*$I$45+C47*$I$46+D47*$I$47+E47*$I$48+F47*$I$49+G47*$I$50</f>
-        <v>0.4318</v>
+        <v>0.02032</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="48">
-      <c r="A48" s="34" t="s">
+      <c r="A48" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="35" t="n">
+      <c r="B48" s="41" t="n">
         <f aca="false">ForwardKinematics!$E$37</f>
         <v>0</v>
       </c>
-      <c r="C48" s="36" t="n">
+      <c r="C48" s="42" t="n">
         <f aca="false">ForwardKinematics!$E$38</f>
         <v>0</v>
       </c>
-      <c r="D48" s="36" t="n">
+      <c r="D48" s="42" t="n">
         <f aca="false">ForwardKinematics!$E$39</f>
         <v>0</v>
       </c>
-      <c r="E48" s="36" t="n">
+      <c r="E48" s="42" t="n">
         <f aca="false">ForwardKinematics!$E$40</f>
-        <v>-1</v>
-      </c>
-      <c r="F48" s="36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F48" s="42" t="n">
         <f aca="false">ForwardKinematics!$E$41</f>
         <v>0</v>
       </c>
-      <c r="G48" s="37" t="n">
+      <c r="G48" s="43" t="n">
         <f aca="false">ForwardKinematics!$E$42</f>
-        <v>-1</v>
-      </c>
-      <c r="I48" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J48" s="39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J48" s="45" t="n">
         <f aca="false">B48*$I$45+C48*$I$46+D48*$I$47+E48*$I$48+F48*$I$49+G48*$I$50</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="49">
-      <c r="A49" s="34"/>
-      <c r="B49" s="35" t="n">
+      <c r="A49" s="40"/>
+      <c r="B49" s="41" t="n">
         <f aca="false">ForwardKinematics!$F$37</f>
         <v>0</v>
       </c>
-      <c r="C49" s="36" t="n">
+      <c r="C49" s="42" t="n">
         <f aca="false">ForwardKinematics!$F$38</f>
         <v>1</v>
       </c>
-      <c r="D49" s="36" t="n">
+      <c r="D49" s="42" t="n">
         <f aca="false">ForwardKinematics!$F$39</f>
         <v>1</v>
       </c>
-      <c r="E49" s="36" t="n">
+      <c r="E49" s="42" t="n">
         <f aca="false">ForwardKinematics!$F$40</f>
         <v>0</v>
       </c>
-      <c r="F49" s="36" t="n">
+      <c r="F49" s="42" t="n">
         <f aca="false">ForwardKinematics!$F$41</f>
         <v>1</v>
       </c>
-      <c r="G49" s="37" t="n">
+      <c r="G49" s="43" t="n">
         <f aca="false">ForwardKinematics!$F$42</f>
         <v>0</v>
       </c>
-      <c r="I49" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J49" s="39" t="n">
+      <c r="I49" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" s="45" t="n">
         <f aca="false">B49*$I$45+C49*$I$46+D49*$I$47+E49*$I$48+F49*$I$49+G49*$I$50</f>
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="50">
-      <c r="A50" s="34"/>
-      <c r="B50" s="40" t="n">
+      <c r="A50" s="40"/>
+      <c r="B50" s="46" t="n">
         <f aca="false">ForwardKinematics!$G$37</f>
         <v>1</v>
       </c>
-      <c r="C50" s="41" t="n">
+      <c r="C50" s="47" t="n">
         <f aca="false">ForwardKinematics!$G$38</f>
         <v>0</v>
       </c>
-      <c r="D50" s="41" t="n">
+      <c r="D50" s="47" t="n">
         <f aca="false">ForwardKinematics!$G$39</f>
         <v>0</v>
       </c>
-      <c r="E50" s="41" t="n">
+      <c r="E50" s="47" t="n">
         <f aca="false">ForwardKinematics!$G$40</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="F50" s="41" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" s="47" t="n">
         <f aca="false">ForwardKinematics!$G$41</f>
         <v>0</v>
       </c>
-      <c r="G50" s="42" t="n">
+      <c r="G50" s="48" t="n">
         <f aca="false">ForwardKinematics!$G$42</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="I50" s="38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J50" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I50" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" s="45" t="n">
         <f aca="false">B50*$I$45+C50*$I$46+D50*$I$47+E50*$I$48+F50*$I$49+G50*$I$50</f>
         <v>0</v>
       </c>
@@ -2136,458 +2196,458 @@
       <c r="E51" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="52">
-      <c r="A52" s="43" t="str">
+      <c r="A52" s="49" t="str">
         <f aca="false">ForwardKinematics!$A$23</f>
         <v>01T</v>
       </c>
-      <c r="B52" s="44" t="n">
+      <c r="B52" s="50" t="n">
         <f aca="false">ForwardKinematics!$B$23</f>
         <v>1</v>
       </c>
-      <c r="C52" s="44" t="n">
+      <c r="C52" s="50" t="n">
         <f aca="false">ForwardKinematics!$C$23</f>
         <v>-0</v>
       </c>
-      <c r="D52" s="44" t="n">
+      <c r="D52" s="50" t="n">
         <f aca="false">ForwardKinematics!$D$23</f>
         <v>0</v>
       </c>
-      <c r="E52" s="45" t="n">
+      <c r="E52" s="51" t="n">
         <f aca="false">ForwardKinematics!$K$23</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="53">
-      <c r="A53" s="43"/>
-      <c r="B53" s="46" t="n">
+      <c r="A53" s="49"/>
+      <c r="B53" s="52" t="n">
         <f aca="false">ForwardKinematics!$E$23</f>
         <v>0</v>
       </c>
-      <c r="C53" s="46" t="n">
+      <c r="C53" s="52" t="n">
         <f aca="false">ForwardKinematics!$F$23</f>
         <v>1</v>
       </c>
-      <c r="D53" s="46" t="n">
+      <c r="D53" s="52" t="n">
         <f aca="false">ForwardKinematics!$G$23</f>
         <v>0</v>
       </c>
-      <c r="E53" s="47" t="n">
+      <c r="E53" s="53" t="n">
         <f aca="false">ForwardKinematics!$L$23</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="54">
-      <c r="A54" s="43"/>
-      <c r="B54" s="48" t="n">
+      <c r="A54" s="49"/>
+      <c r="B54" s="54" t="n">
         <f aca="false">ForwardKinematics!$H$23</f>
         <v>0</v>
       </c>
-      <c r="C54" s="48" t="n">
+      <c r="C54" s="54" t="n">
         <f aca="false">ForwardKinematics!$I$23</f>
         <v>0</v>
       </c>
-      <c r="D54" s="48" t="n">
+      <c r="D54" s="54" t="n">
         <f aca="false">ForwardKinematics!$J$23</f>
         <v>1</v>
       </c>
-      <c r="E54" s="47" t="n">
+      <c r="E54" s="53" t="n">
         <f aca="false">ForwardKinematics!$M$23</f>
         <v>0.674</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="55">
-      <c r="A55" s="43"/>
-      <c r="B55" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C55" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" s="50" t="n">
+      <c r="A55" s="49"/>
+      <c r="B55" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" s="56" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="56">
-      <c r="A56" s="43" t="str">
+      <c r="A56" s="49" t="str">
         <f aca="false">ForwardKinematics!$A$24</f>
         <v>02T</v>
       </c>
-      <c r="B56" s="44" t="n">
+      <c r="B56" s="50" t="n">
         <f aca="false">ForwardKinematics!$B$24</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C56" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C56" s="50" t="n">
         <f aca="false">ForwardKinematics!$C$24</f>
         <v>0</v>
       </c>
-      <c r="D56" s="44" t="n">
+      <c r="D56" s="50" t="n">
         <f aca="false">ForwardKinematics!$D$24</f>
-        <v>-1</v>
-      </c>
-      <c r="E56" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" s="51" t="n">
         <f aca="false">ForwardKinematics!$K$24</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="57">
-      <c r="A57" s="43"/>
-      <c r="B57" s="46" t="n">
+      <c r="A57" s="49"/>
+      <c r="B57" s="52" t="n">
         <f aca="false">ForwardKinematics!$E$24</f>
         <v>0</v>
       </c>
-      <c r="C57" s="46" t="n">
+      <c r="C57" s="52" t="n">
         <f aca="false">ForwardKinematics!$F$24</f>
         <v>1</v>
       </c>
-      <c r="D57" s="46" t="n">
+      <c r="D57" s="52" t="n">
         <f aca="false">ForwardKinematics!$G$24</f>
         <v>0</v>
       </c>
-      <c r="E57" s="47" t="n">
+      <c r="E57" s="53" t="n">
         <f aca="false">ForwardKinematics!$L$24</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="58">
-      <c r="A58" s="43"/>
-      <c r="B58" s="48" t="n">
+      <c r="A58" s="49"/>
+      <c r="B58" s="54" t="n">
         <f aca="false">ForwardKinematics!$H$24</f>
-        <v>1</v>
-      </c>
-      <c r="C58" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" s="54" t="n">
         <f aca="false">ForwardKinematics!$I$24</f>
         <v>0</v>
       </c>
-      <c r="D58" s="48" t="n">
+      <c r="D58" s="54" t="n">
         <f aca="false">ForwardKinematics!$J$24</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="E58" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" s="53" t="n">
         <f aca="false">ForwardKinematics!$M$24</f>
         <v>0.674</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="59">
-      <c r="A59" s="43"/>
-      <c r="B59" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C59" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D59" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E59" s="50" t="n">
+      <c r="A59" s="49"/>
+      <c r="B59" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" s="56" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="60">
-      <c r="A60" s="43" t="str">
+      <c r="A60" s="49" t="str">
         <f aca="false">ForwardKinematics!$A$25</f>
         <v>03T</v>
       </c>
-      <c r="B60" s="44" t="n">
+      <c r="B60" s="50" t="n">
         <f aca="false">ForwardKinematics!$B$25</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C60" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C60" s="50" t="n">
         <f aca="false">ForwardKinematics!$C$25</f>
         <v>0</v>
       </c>
-      <c r="D60" s="44" t="n">
+      <c r="D60" s="50" t="n">
         <f aca="false">ForwardKinematics!$D$25</f>
-        <v>-1</v>
-      </c>
-      <c r="E60" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" s="51" t="n">
         <f aca="false">ForwardKinematics!$K$25</f>
-        <v>2.64401243935914E-017</v>
+        <v>0.4318</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="61">
-      <c r="A61" s="43"/>
-      <c r="B61" s="46" t="n">
+      <c r="A61" s="49"/>
+      <c r="B61" s="52" t="n">
         <f aca="false">ForwardKinematics!$E$25</f>
         <v>0</v>
       </c>
-      <c r="C61" s="46" t="n">
+      <c r="C61" s="52" t="n">
         <f aca="false">ForwardKinematics!$F$25</f>
         <v>1</v>
       </c>
-      <c r="D61" s="46" t="n">
+      <c r="D61" s="52" t="n">
         <f aca="false">ForwardKinematics!$G$25</f>
         <v>0</v>
       </c>
-      <c r="E61" s="47" t="n">
+      <c r="E61" s="53" t="n">
         <f aca="false">ForwardKinematics!$L$25</f>
         <v>0.12446</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="62">
-      <c r="A62" s="43"/>
-      <c r="B62" s="48" t="n">
+      <c r="A62" s="49"/>
+      <c r="B62" s="54" t="n">
         <f aca="false">ForwardKinematics!$H$25</f>
-        <v>1</v>
-      </c>
-      <c r="C62" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" s="54" t="n">
         <f aca="false">ForwardKinematics!$I$25</f>
         <v>0</v>
       </c>
-      <c r="D62" s="48" t="n">
+      <c r="D62" s="54" t="n">
         <f aca="false">ForwardKinematics!$J$25</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="E62" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E62" s="53" t="n">
         <f aca="false">ForwardKinematics!$M$25</f>
-        <v>1.1058</v>
+        <v>0.674</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="63">
-      <c r="A63" s="43"/>
-      <c r="B63" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C63" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D63" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E63" s="50" t="n">
+      <c r="A63" s="49"/>
+      <c r="B63" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C63" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E63" s="56" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="64">
-      <c r="A64" s="43" t="str">
+      <c r="A64" s="49" t="str">
         <f aca="false">ForwardKinematics!$A$26</f>
         <v>04T</v>
       </c>
-      <c r="B64" s="44" t="n">
+      <c r="B64" s="50" t="n">
         <f aca="false">ForwardKinematics!$B$26</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C64" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C64" s="50" t="n">
         <f aca="false">ForwardKinematics!$C$26</f>
         <v>0</v>
       </c>
-      <c r="D64" s="44" t="n">
+      <c r="D64" s="50" t="n">
         <f aca="false">ForwardKinematics!$D$26</f>
-        <v>-1</v>
-      </c>
-      <c r="E64" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E64" s="51" t="n">
         <f aca="false">ForwardKinematics!$K$26</f>
-        <v>-0.4318</v>
+        <v>0.41148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="65">
-      <c r="A65" s="43"/>
-      <c r="B65" s="46" t="n">
+      <c r="A65" s="49"/>
+      <c r="B65" s="52" t="n">
         <f aca="false">ForwardKinematics!$E$26</f>
         <v>0</v>
       </c>
-      <c r="C65" s="46" t="n">
+      <c r="C65" s="52" t="n">
         <f aca="false">ForwardKinematics!$F$26</f>
         <v>1</v>
       </c>
-      <c r="D65" s="46" t="n">
+      <c r="D65" s="52" t="n">
         <f aca="false">ForwardKinematics!$G$26</f>
         <v>0</v>
       </c>
-      <c r="E65" s="47" t="n">
+      <c r="E65" s="53" t="n">
         <f aca="false">ForwardKinematics!$L$26</f>
         <v>0.12446</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="66">
-      <c r="A66" s="43"/>
-      <c r="B66" s="48" t="n">
+      <c r="A66" s="49"/>
+      <c r="B66" s="54" t="n">
         <f aca="false">ForwardKinematics!$H$26</f>
-        <v>1</v>
-      </c>
-      <c r="C66" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C66" s="54" t="n">
         <f aca="false">ForwardKinematics!$I$26</f>
         <v>0</v>
       </c>
-      <c r="D66" s="48" t="n">
+      <c r="D66" s="54" t="n">
         <f aca="false">ForwardKinematics!$J$26</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="E66" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="53" t="n">
         <f aca="false">ForwardKinematics!$M$26</f>
-        <v>1.08548</v>
+        <v>1.1058</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="67">
-      <c r="A67" s="43"/>
-      <c r="B67" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C67" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D67" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E67" s="50" t="n">
+      <c r="A67" s="49"/>
+      <c r="B67" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C67" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D67" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E67" s="56" t="n">
         <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="68">
-      <c r="A68" s="43" t="str">
+      <c r="A68" s="49" t="str">
         <f aca="false">ForwardKinematics!$A$27</f>
         <v>05T</v>
       </c>
-      <c r="B68" s="44" t="n">
+      <c r="B68" s="50" t="n">
         <f aca="false">ForwardKinematics!$B$27</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C68" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C68" s="50" t="n">
         <f aca="false">ForwardKinematics!$C$27</f>
         <v>0</v>
       </c>
-      <c r="D68" s="44" t="n">
+      <c r="D68" s="50" t="n">
         <f aca="false">ForwardKinematics!$D$27</f>
-        <v>-1</v>
-      </c>
-      <c r="E68" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E68" s="51" t="n">
         <f aca="false">ForwardKinematics!$K$27</f>
-        <v>-0.4318</v>
+        <v>0.41148</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="69">
-      <c r="A69" s="43"/>
-      <c r="B69" s="46" t="n">
+      <c r="A69" s="49"/>
+      <c r="B69" s="52" t="n">
         <f aca="false">ForwardKinematics!$E$27</f>
         <v>0</v>
       </c>
-      <c r="C69" s="46" t="n">
+      <c r="C69" s="52" t="n">
         <f aca="false">ForwardKinematics!$F$27</f>
         <v>1</v>
       </c>
-      <c r="D69" s="46" t="n">
+      <c r="D69" s="52" t="n">
         <f aca="false">ForwardKinematics!$G$27</f>
         <v>0</v>
       </c>
-      <c r="E69" s="47" t="n">
+      <c r="E69" s="53" t="n">
         <f aca="false">ForwardKinematics!$L$27</f>
         <v>0.12446</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="70">
-      <c r="A70" s="43"/>
-      <c r="B70" s="48" t="n">
+      <c r="A70" s="49"/>
+      <c r="B70" s="54" t="n">
         <f aca="false">ForwardKinematics!$H$27</f>
-        <v>1</v>
-      </c>
-      <c r="C70" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C70" s="54" t="n">
         <f aca="false">ForwardKinematics!$I$27</f>
         <v>0</v>
       </c>
-      <c r="D70" s="48" t="n">
+      <c r="D70" s="54" t="n">
         <f aca="false">ForwardKinematics!$J$27</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="E70" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E70" s="53" t="n">
         <f aca="false">ForwardKinematics!$M$27</f>
-        <v>1.08548</v>
+        <v>1.1058</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="71">
-      <c r="A71" s="43"/>
-      <c r="B71" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C71" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D71" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E71" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="I71" s="30" t="s">
+      <c r="A71" s="49"/>
+      <c r="B71" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C71" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D71" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E71" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="I71" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="J71" s="30"/>
+      <c r="J71" s="36"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="72">
-      <c r="A72" s="43" t="str">
+      <c r="A72" s="49" t="str">
         <f aca="false">ForwardKinematics!$A$28</f>
         <v>06T</v>
       </c>
-      <c r="B72" s="44" t="n">
+      <c r="B72" s="50" t="n">
         <f aca="false">ForwardKinematics!$B$28</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C72" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C72" s="50" t="n">
         <f aca="false">ForwardKinematics!$C$28</f>
         <v>0</v>
       </c>
-      <c r="D72" s="44" t="n">
+      <c r="D72" s="50" t="n">
         <f aca="false">ForwardKinematics!$D$28</f>
-        <v>-1</v>
-      </c>
-      <c r="E72" s="45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E72" s="51" t="n">
         <f aca="false">ForwardKinematics!$K$28</f>
-        <v>-0.4318</v>
-      </c>
-      <c r="I72" s="51" t="s">
+        <v>0.41148</v>
+      </c>
+      <c r="I72" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="J72" s="26" t="n">
+      <c r="J72" s="34" t="n">
         <f aca="false">(C74-D73)/4/J75</f>
         <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="73">
-      <c r="A73" s="43"/>
-      <c r="B73" s="46" t="n">
+      <c r="A73" s="49"/>
+      <c r="B73" s="52" t="n">
         <f aca="false">ForwardKinematics!$E$28</f>
         <v>0</v>
       </c>
-      <c r="C73" s="46" t="n">
+      <c r="C73" s="52" t="n">
         <f aca="false">ForwardKinematics!$F$28</f>
         <v>1</v>
       </c>
-      <c r="D73" s="46" t="n">
+      <c r="D73" s="52" t="n">
         <f aca="false">ForwardKinematics!$G$28</f>
         <v>0</v>
       </c>
-      <c r="E73" s="47" t="n">
+      <c r="E73" s="53" t="n">
         <f aca="false">ForwardKinematics!$L$28</f>
         <v>0.12446</v>
       </c>
-      <c r="I73" s="52" t="s">
+      <c r="I73" s="58" t="s">
         <v>50</v>
       </c>
       <c r="J73" s="7" t="n">
         <f aca="false">(D72-B74)/4/J75</f>
-        <v>-0.707106781186547</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="74">
-      <c r="A74" s="43"/>
-      <c r="B74" s="48" t="n">
+      <c r="A74" s="49"/>
+      <c r="B74" s="54" t="n">
         <f aca="false">ForwardKinematics!$H$28</f>
-        <v>1</v>
-      </c>
-      <c r="C74" s="48" t="n">
+        <v>0</v>
+      </c>
+      <c r="C74" s="54" t="n">
         <f aca="false">ForwardKinematics!$I$28</f>
         <v>0</v>
       </c>
-      <c r="D74" s="48" t="n">
+      <c r="D74" s="54" t="n">
         <f aca="false">ForwardKinematics!$J$28</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="E74" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E74" s="53" t="n">
         <f aca="false">ForwardKinematics!$M$28</f>
-        <v>1.08548</v>
-      </c>
-      <c r="I74" s="52" t="s">
+        <v>1.1058</v>
+      </c>
+      <c r="I74" s="58" t="s">
         <v>51</v>
       </c>
       <c r="J74" s="7" t="n">
@@ -2596,25 +2656,25 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="75">
-      <c r="A75" s="43"/>
-      <c r="B75" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="C75" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D75" s="49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E75" s="50" t="n">
-        <v>1</v>
-      </c>
-      <c r="I75" s="53" t="s">
+      <c r="A75" s="49"/>
+      <c r="B75" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="C75" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D75" s="55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E75" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="I75" s="59" t="s">
         <v>52</v>
       </c>
       <c r="J75" s="14" t="n">
         <f aca="false">0.5*SQRT(1+B72+C73+D74)</f>
-        <v>0.707106781186548</v>
+        <v>1</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="76">
@@ -2625,27 +2685,27 @@
       <c r="C76" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="77">
-      <c r="A77" s="54" t="s">
+      <c r="A77" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="B77" s="24" t="n">
+      <c r="B77" s="33" t="n">
         <f aca="false">C74-D73</f>
         <v>0</v>
       </c>
-      <c r="C77" s="26"/>
+      <c r="C77" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="78">
-      <c r="A78" s="55" t="s">
+      <c r="A78" s="61" t="s">
         <v>55</v>
       </c>
       <c r="B78" s="0" t="n">
         <f aca="false">D72-B74</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="C78" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="79">
-      <c r="A79" s="55" t="s">
+      <c r="A79" s="61" t="s">
         <v>56</v>
       </c>
       <c r="B79" s="0" t="n">
@@ -2655,74 +2715,74 @@
       <c r="C79" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="80">
-      <c r="A80" s="55" t="s">
+      <c r="A80" s="61" t="s">
         <v>57</v>
       </c>
       <c r="B80" s="0" t="n">
         <f aca="false">SQRT(B77^2+B78^2+B79^2)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C80" s="7"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="81">
-      <c r="A81" s="55" t="s">
+      <c r="A81" s="61" t="s">
         <v>58</v>
       </c>
       <c r="B81" s="0" t="n">
         <f aca="false">B72+C73+D74</f>
-        <v>1</v>
-      </c>
-      <c r="C81" s="56" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="62" t="s">
         <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="82">
-      <c r="A82" s="55" t="s">
+      <c r="A82" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="B82" s="57" t="n">
+      <c r="B82" s="63" t="n">
         <f aca="false">ATAN2(B81-1,B80)</f>
-        <v>1.5707963267949</v>
-      </c>
-      <c r="C82" s="56"/>
+        <v>0</v>
+      </c>
+      <c r="C82" s="62"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.35" outlineLevel="0" r="83">
-      <c r="A83" s="55" t="s">
+      <c r="A83" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B83" s="57" t="n">
+      <c r="B83" s="63" t="e">
         <f aca="false">B77/$B$80</f>
-        <v>0</v>
-      </c>
-      <c r="C83" s="58" t="n">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C83" s="64" t="e">
         <f aca="false">B83*$B$82</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="84">
-      <c r="A84" s="55" t="s">
+      <c r="A84" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="B84" s="57" t="n">
+      <c r="B84" s="63" t="e">
         <f aca="false">B78/$B$80</f>
-        <v>-1</v>
-      </c>
-      <c r="C84" s="58" t="n">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C84" s="64" t="e">
         <f aca="false">B84*$B$82</f>
-        <v>-1.5707963267949</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.35" outlineLevel="0" r="85">
-      <c r="A85" s="59" t="s">
+      <c r="A85" s="65" t="s">
         <v>63</v>
       </c>
-      <c r="B85" s="60" t="n">
+      <c r="B85" s="66" t="e">
         <f aca="false">B79/$B$80</f>
-        <v>0</v>
-      </c>
-      <c r="C85" s="61" t="n">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C85" s="67" t="e">
         <f aca="false">B85*$B$82</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="86">
@@ -2733,45 +2793,45 @@
       <c r="D86" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="87">
-      <c r="B87" s="25" t="n">
+      <c r="B87" s="68" t="e">
         <f aca="false">$B$83^2*(1-COS($B$82))+COS($B$82)</f>
-        <v>6.12323399573677E-017</v>
-      </c>
-      <c r="C87" s="24" t="n">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C87" s="33" t="e">
         <f aca="false">$B$83*$B$84*(1-COS($B$82))-$B$85*SIN($B$82)</f>
-        <v>-0</v>
-      </c>
-      <c r="D87" s="26" t="n">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D87" s="34" t="e">
         <f aca="false">$B$83*$B$85*(1-COS($B$82))+$B$84*SIN($B$82)</f>
-        <v>-1</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="88">
-      <c r="B88" s="27" t="n">
+      <c r="B88" s="69" t="e">
         <f aca="false">$B$83*$B$84*(1-COS($B$82))+$B$85*SIN($B$82)</f>
-        <v>0</v>
-      </c>
-      <c r="C88" s="0" t="n">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C88" s="0" t="e">
         <f aca="false">$B$84^2*(1-COS($B$82))+COS($B$82)</f>
-        <v>1</v>
-      </c>
-      <c r="D88" s="7" t="n">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D88" s="7" t="e">
         <f aca="false">$B$84*$B$85*(1-COS($B$82))-$B$83*SIN($B$82)</f>
-        <v>-0</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="89">
-      <c r="B89" s="28" t="n">
+      <c r="B89" s="70" t="e">
         <f aca="false">$B$83*$B$85*(1-COS($B$82))-$B$84*SIN($B$82)</f>
-        <v>1</v>
-      </c>
-      <c r="C89" s="12" t="n">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C89" s="12" t="e">
         <f aca="false">$B$84*$B$85*(1-COS($B$82))+$B$83*SIN($B$82)</f>
-        <v>0</v>
-      </c>
-      <c r="D89" s="14" t="n">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D89" s="14" t="e">
         <f aca="false">$B$85^2*(1-COS($B$82))+COS($B$82)</f>
-        <v>6.12323399573677E-017</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -2817,97 +2877,97 @@
   </sheetPr>
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100">
-      <selection activeCell="D8" activeCellId="0" pane="topLeft" sqref="D8"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+      <selection activeCell="I21" activeCellId="0" pane="topLeft" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.9333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="75.3019607843137"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="71" t="s">
         <v>65</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="2">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="71" t="s">
         <v>66</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="3">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="71" t="s">
         <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="4">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="71" t="s">
         <v>68</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="62" t="s">
+      <c r="A5" s="71" t="s">
         <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="6">
-      <c r="A6" s="62" t="s">
+      <c r="A6" s="71" t="s">
         <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="71" t="s">
         <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="A8" s="62" t="s">
+      <c r="A8" s="71" t="s">
         <v>71</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="A9" s="62" t="s">
+      <c r="A9" s="71" t="s">
         <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="71" t="s">
         <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="71" t="s">
         <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="A12" s="62" t="s">
+      <c r="A12" s="71" t="s">
         <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="71" t="s">
         <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="71" t="s">
         <v>75</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="71" t="s">
         <v>76</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
-      <c r="A16" s="62" t="s">
+      <c r="A16" s="71" t="s">
         <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="71" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2919,5 +2979,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>